<commit_message>
Fix the signed languages
</commit_message>
<xml_diff>
--- a/resources/lang/Langues.xlsx
+++ b/resources/lang/Langues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Ecole\Q5\PRJG5\gmi\resources\lang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Snow\Desktop\gmi\resources\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817AB6F9-87D9-445B-821B-04E416BEDA31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E03EA11-4349-452C-8A5F-0BB8591FBCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="4095" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -361,29 +361,29 @@
     <t>Langue des signes francophone de Belgique</t>
   </si>
   <si>
-    <t>SFB</t>
-  </si>
-  <si>
-    <t>Langue des signes néerlandophone de Belgique</t>
-  </si>
-  <si>
     <t>VGT</t>
   </si>
   <si>
     <t>Système des signes international</t>
   </si>
   <si>
-    <t>ILS</t>
-  </si>
-  <si>
     <t>GRE</t>
+  </si>
+  <si>
+    <t>LSBF</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Vlaamse Gevarentaal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -401,6 +401,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,10 +429,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,11 +665,11 @@
   </sheetPr>
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.28515625" customWidth="1"/>
   </cols>
@@ -822,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -1121,21 +1130,21 @@
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>113</v>
+      <c r="B57" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>117</v>
@@ -1151,5 +1160,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>